<commit_message>
korjaa migraatiotesti ja lisaa testeja
</commit_message>
<xml_diff>
--- a/migration-cli/migraatiotesti.xlsx
+++ b/migration-cli/migraatiotesti.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maikol/git/vayla/hassu/migration-cli/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhani/Code/hassu/migration-cli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA65E622-D128-E347-BE9B-E028B727AB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638BF98D-2EA3-9348-9C81-48393A905FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="21900" xr2:uid="{3DE98AE2-DEE6-7943-9A75-A1A5FDC9F021}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="21900" activeTab="1" xr2:uid="{3DE98AE2-DEE6-7943-9A75-A1A5FDC9F021}"/>
   </bookViews>
   <sheets>
     <sheet name="Migraatio" sheetId="1" r:id="rId1"/>
-    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Migraatio2" sheetId="4" r:id="rId2"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>oid</t>
   </si>
@@ -438,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B992D1A-296E-D848-9FFB-954A87184DA3}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -495,18 +496,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44833</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4">
       <c r="D6" s="2"/>
@@ -530,6 +520,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2530CF31-26BF-A441-994A-672C8D661AC7}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44833</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="D3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5F507F3B-287E-CF4F-BC8E-09600F14B306}">
+          <x14:formula1>
+            <xm:f>Metadata!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B9:B1048576 B1:B5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BDFA78-FF4D-1C48-AE61-9505106BD8E1}">
   <dimension ref="A1:A11"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix: muuta migrointiskripti sietämään puutteellisia excel-tiedostoja. Lisää tuki monelle välilehdelle. (#694)
* fix: muuta migrointiskripti sietämään puutteellisia excel-tiedostoja. Lisää tuki monelle välilehdelle.

* korjaa migraatiotesti ja lisaa testeja

---------

Co-authored-by: kettunenj <juhani.kettunen@cgi.com>
</commit_message>
<xml_diff>
--- a/migration-cli/migraatiotesti.xlsx
+++ b/migration-cli/migraatiotesti.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maikol/git/vayla/hassu/migration-cli/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhani/Code/hassu/migration-cli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA65E622-D128-E347-BE9B-E028B727AB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638BF98D-2EA3-9348-9C81-48393A905FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="21900" xr2:uid="{3DE98AE2-DEE6-7943-9A75-A1A5FDC9F021}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="21900" activeTab="1" xr2:uid="{3DE98AE2-DEE6-7943-9A75-A1A5FDC9F021}"/>
   </bookViews>
   <sheets>
     <sheet name="Migraatio" sheetId="1" r:id="rId1"/>
-    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Migraatio2" sheetId="4" r:id="rId2"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>oid</t>
   </si>
@@ -438,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B992D1A-296E-D848-9FFB-954A87184DA3}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -495,18 +496,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44833</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4">
       <c r="D6" s="2"/>
@@ -530,6 +520,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2530CF31-26BF-A441-994A-672C8D661AC7}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44833</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="D3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5F507F3B-287E-CF4F-BC8E-09600F14B306}">
+          <x14:formula1>
+            <xm:f>Metadata!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B9:B1048576 B1:B5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BDFA78-FF4D-1C48-AE61-9505106BD8E1}">
   <dimension ref="A1:A11"/>
   <sheetViews>

</xml_diff>